<commit_message>
Quick data update to attempt to enforce the float type on the lat/lon cols
</commit_message>
<xml_diff>
--- a/Madelaine_Gerald/data/Demand_Node_Data.xlsx
+++ b/Madelaine_Gerald/data/Demand_Node_Data.xlsx
@@ -8535,10 +8535,8 @@
       <c r="E270" t="n">
         <v>8.5122</v>
       </c>
-      <c r="F270" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> -81.3626</t>
-        </is>
+      <c r="F270" t="n">
+        <v>-81.3626</v>
       </c>
       <c r="G270" t="n">
         <v>885.948</v>
@@ -8927,10 +8925,8 @@
       <c r="E283" t="n">
         <v>8.916764000000001</v>
       </c>
-      <c r="F283" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> -79.883671</t>
-        </is>
+      <c r="F283" t="n">
+        <v>-79.88367100000001</v>
       </c>
       <c r="G283" t="n">
         <v>954.603</v>
@@ -13189,10 +13185,8 @@
       <c r="E425" t="n">
         <v>8.33333</v>
       </c>
-      <c r="F425" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> -81.5667</t>
-        </is>
+      <c r="F425" t="n">
+        <v>-81.5667</v>
       </c>
       <c r="G425" t="n">
         <v>1510.41</v>
@@ -14091,10 +14085,8 @@
       <c r="E455" t="n">
         <v>8.942269</v>
       </c>
-      <c r="F455" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> -78.91155</t>
-        </is>
+      <c r="F455" t="n">
+        <v>-78.91155000000001</v>
       </c>
       <c r="G455" t="n">
         <v>274.023</v>
@@ -15053,10 +15045,8 @@
       <c r="E487" t="n">
         <v>8.183142999999999</v>
       </c>
-      <c r="F487" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> -80.682588</t>
-        </is>
+      <c r="F487" t="n">
+        <v>-80.682588</v>
       </c>
       <c r="G487" t="n">
         <v>2420.835</v>

</xml_diff>